<commit_message>
add update save feature
</commit_message>
<xml_diff>
--- a/Financial-1402-1.xlsx
+++ b/Financial-1402-1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="save" sheetId="1" state="visible" r:id="rId1"/>
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>sum</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -498,10 +503,11 @@
       <c r="D2" t="n">
         <v>31</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2000</t>
-        </is>
+      <c r="E2" t="n">
+        <v>9000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -515,7 +521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +540,11 @@
           <t>desc</t>
         </is>
       </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -541,8 +552,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>taxi</t>
-        </is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add date and time to save & save_log
</commit_message>
<xml_diff>
--- a/Financial-1402-1.xlsx
+++ b/Financial-1402-1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="save" sheetId="1" state="visible" r:id="rId1"/>
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,53 +461,63 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
           <t>month_id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>week_id</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>day_id</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>sum</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>id</t>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>date</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>6</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>31</v>
       </c>
-      <c r="E2" t="n">
-        <v>9000</v>
-      </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>8000</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1402/06/31</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -521,7 +531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,6 +555,11 @@
           <t>amount</t>
         </is>
       </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -552,11 +567,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>texi</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6000</v>
+        <v>5000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -565,11 +585,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>bazi</t>
         </is>
       </c>
       <c r="C3" t="n">
         <v>3000</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>19:35</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix total table save & cost fields
</commit_message>
<xml_diff>
--- a/Financial-1402-1.xlsx
+++ b/Financial-1402-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\Programing\BootStrap Ex\python\financial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E65412-54AC-40E7-811F-ED7F35957E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100DFE4E-5758-4809-99BC-72A2BD090686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,18 +75,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -102,7 +97,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,31 +120,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -463,25 +440,25 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -495,25 +472,25 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -565,7 +542,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,7 +571,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -603,22 +580,23 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add SELECT_TABLE function to app, fix updating total sheet during update other sheets(save or log)
</commit_message>
<xml_diff>
--- a/Financial-1402-1.xlsx
+++ b/Financial-1402-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\Programing\BootStrap Ex\python\financial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100DFE4E-5758-4809-99BC-72A2BD090686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675F7591-A529-427E-9A56-E5450EF028F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="save" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -97,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,13 +125,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -433,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -471,9 +494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -510,25 +531,25 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -542,25 +563,25 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -570,34 +591,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEBD4B2-6DB1-41D8-9C04-946E032553B2}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add youtube url video to README
</commit_message>
<xml_diff>
--- a/Financial-1402-1.xlsx
+++ b/Financial-1402-1.xlsx
@@ -1,108 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\parham\Programing\BootStrap Ex\python\financial\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CD7DA1-878E-45F0-8CD8-ED2FAB29B997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="save" sheetId="1" r:id="rId1"/>
-    <sheet name="save_log" sheetId="2" r:id="rId2"/>
-    <sheet name="cost" sheetId="3" r:id="rId3"/>
-    <sheet name="cost_log" sheetId="4" r:id="rId4"/>
-    <sheet name="total" sheetId="5" r:id="rId5"/>
+    <sheet name="save" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="save_log" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="cost" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="cost_log" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="total" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>month_id</t>
-  </si>
-  <si>
-    <t>week_id</t>
-  </si>
-  <si>
-    <t>day_id</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>sum</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>save_id</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>cost_id</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>cost</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -140,32 +88,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -453,36 +469,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>month_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>week_id</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>day_id</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="D2" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
+      <c r="E2" t="n">
+        <v>13</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1402/07/13</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -491,30 +550,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>save_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>desc</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>taxi</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>game</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>20:42</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -523,36 +638,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>month_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>week_id</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>day_id</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>sum</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D2" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="E2" t="n">
+        <v>13</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1402/07/13</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -561,30 +719,65 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>cost_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>desc</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>buy something</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20:43</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -593,30 +786,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>month_id</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>save</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
+      <c r="B2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1402</v>
+      </c>
+      <c r="D2" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>